<commit_message>
Edit EXCEL AND XLML file
</commit_message>
<xml_diff>
--- a/TM/TestApp/_Files/Exel/TM.xlsx
+++ b/TM/TestApp/_Files/Exel/TM.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26827"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2EE74083-AB1C-45D3-87B2-493217588095}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{553B02C8-F966-4CB8-87D6-7A7C33A8BAA5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4665" yWindow="3015" windowWidth="15375" windowHeight="7785" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TestResult" sheetId="1" r:id="rId1"/>
@@ -20,86 +20,29 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
   <si>
     <t>سریال دستگاه ها</t>
   </si>
   <si>
-    <t>ارتباط سریال RS485</t>
-  </si>
-  <si>
-    <t>ارتباط سریال OP</t>
-  </si>
-  <si>
-    <t>پروگرم برنامه نهایی</t>
-  </si>
-  <si>
-    <t>ورژن سخت افزار تستر</t>
-  </si>
-  <si>
     <t xml:space="preserve"> ورژن نرم افزار تستر</t>
   </si>
   <si>
-    <t>نسخه نرم افزار با استند تست</t>
-  </si>
-  <si>
     <t>ExcelCheckSumA</t>
   </si>
   <si>
     <t>ExcelCheckSumB</t>
   </si>
   <si>
-    <t>چاپ اطلاعات تست</t>
-  </si>
-  <si>
     <t>Version</t>
   </si>
   <si>
     <t>ولتاژ 3.3 ولت</t>
   </si>
   <si>
-    <t>تست برد با نرم افزار</t>
-  </si>
-  <si>
     <t xml:space="preserve">اتصال تغذیه 12 ولت </t>
   </si>
   <si>
-    <t>LED Power</t>
-  </si>
-  <si>
-    <t>LED RS485</t>
-  </si>
-  <si>
-    <t>LED Net 1</t>
-  </si>
-  <si>
-    <t>LED Net 2</t>
-  </si>
-  <si>
-    <t>ولتاژ GSM</t>
-  </si>
-  <si>
-    <t>ولتاژ GSM EXT</t>
-  </si>
-  <si>
-    <t>ولتاژ باتری ساعت</t>
-  </si>
-  <si>
-    <t>ولتاژ مدار RTC</t>
-  </si>
-  <si>
-    <t>مدار کلید دریست</t>
-  </si>
-  <si>
-    <t>مدار کلید کارخانه</t>
-  </si>
-  <si>
-    <t>عملکرد فلش خارجی</t>
-  </si>
-  <si>
-    <t>ارتباط ماژول مودم</t>
-  </si>
-  <si>
     <t>تنظیمات اعمال شده</t>
   </si>
   <si>
@@ -109,16 +52,25 @@
     <t>بررسی مدار Zero Cross</t>
   </si>
   <si>
-    <t>OK</t>
-  </si>
-  <si>
-    <t>v1.14011007</t>
-  </si>
-  <si>
-    <t>5E372FF69D5910ECC0D3049A250E6B48</t>
-  </si>
-  <si>
-    <t>Time = [1402/06/18 09:57:26] Device = [00310212345678] Domain = [94.139.169.122:8000]</t>
+    <t>LED</t>
+  </si>
+  <si>
+    <t>ولتاژ باتری</t>
+  </si>
+  <si>
+    <t>ارتباط سریال</t>
+  </si>
+  <si>
+    <t>کلید</t>
+  </si>
+  <si>
+    <t>حافظه خارجی</t>
+  </si>
+  <si>
+    <t>ولتاز مودم</t>
+  </si>
+  <si>
+    <t>عملکرد مودم</t>
   </si>
 </sst>
 </file>
@@ -169,7 +121,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="7">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -215,19 +167,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
       <top style="medium">
@@ -255,7 +194,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -286,9 +225,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -571,164 +507,108 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:CP4"/>
+  <dimension ref="A1:CE4"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="G11" sqref="G11"/>
+      <selection pane="topRight" activeCell="Q8" sqref="Q8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="26.140625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="16.28515625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="14.5703125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="21.140625" style="1" customWidth="1"/>
-    <col min="5" max="5" width="15.7109375" style="1" customWidth="1"/>
-    <col min="6" max="6" width="10.140625" style="1" customWidth="1"/>
-    <col min="7" max="7" width="9.85546875" style="1" customWidth="1"/>
-    <col min="8" max="9" width="9.28515625" style="1" customWidth="1"/>
-    <col min="10" max="10" width="10.7109375" style="1" customWidth="1"/>
-    <col min="11" max="11" width="8.42578125" style="1" customWidth="1"/>
-    <col min="12" max="12" width="12.5703125" style="1" customWidth="1"/>
-    <col min="13" max="13" width="13" style="1" customWidth="1"/>
-    <col min="14" max="14" width="11" style="1" customWidth="1"/>
-    <col min="15" max="15" width="12.42578125" style="1" customWidth="1"/>
-    <col min="16" max="16" width="15.140625" style="1" customWidth="1"/>
-    <col min="17" max="17" width="12.7109375" style="1" customWidth="1"/>
-    <col min="18" max="18" width="13" style="1" customWidth="1"/>
-    <col min="19" max="19" width="14.85546875" style="1" customWidth="1"/>
-    <col min="20" max="20" width="13.7109375" style="1" customWidth="1"/>
-    <col min="21" max="21" width="85" style="1" customWidth="1"/>
-    <col min="22" max="22" width="17.28515625" style="1" customWidth="1"/>
-    <col min="23" max="23" width="18" style="1" customWidth="1"/>
-    <col min="24" max="24" width="13.85546875" style="1" customWidth="1"/>
-    <col min="25" max="25" width="15.42578125" style="1" customWidth="1"/>
-    <col min="26" max="26" width="16" style="1" customWidth="1"/>
-    <col min="27" max="27" width="37.42578125" style="1" customWidth="1"/>
-    <col min="28" max="28" width="12.5703125" style="1" customWidth="1"/>
-    <col min="94" max="94" width="64" customWidth="1"/>
+    <col min="2" max="2" width="14.5703125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="15.7109375" style="1" customWidth="1"/>
+    <col min="4" max="4" width="10.140625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="10.7109375" style="1" customWidth="1"/>
+    <col min="6" max="6" width="8.42578125" style="1" customWidth="1"/>
+    <col min="7" max="7" width="12.5703125" style="1" customWidth="1"/>
+    <col min="8" max="8" width="13" style="1" customWidth="1"/>
+    <col min="9" max="9" width="11" style="1" customWidth="1"/>
+    <col min="10" max="10" width="12.42578125" style="1" customWidth="1"/>
+    <col min="11" max="11" width="15.140625" style="1" customWidth="1"/>
+    <col min="12" max="12" width="85" style="1" customWidth="1"/>
+    <col min="13" max="13" width="17.28515625" style="1" customWidth="1"/>
+    <col min="14" max="14" width="18" style="1" customWidth="1"/>
+    <col min="15" max="15" width="16" style="1" customWidth="1"/>
+    <col min="16" max="16" width="37.42578125" style="1" customWidth="1"/>
+    <col min="17" max="17" width="12.5703125" style="1" customWidth="1"/>
+    <col min="83" max="83" width="64" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:94" ht="37.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:83" ht="37.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="C1" s="11"/>
-      <c r="D1" s="11"/>
-      <c r="E1" s="11"/>
-      <c r="F1" s="11"/>
-      <c r="G1" s="11"/>
-      <c r="H1" s="11"/>
-      <c r="I1" s="11"/>
-      <c r="J1" s="11"/>
-      <c r="K1" s="11"/>
-      <c r="L1" s="11"/>
-      <c r="M1" s="11"/>
-      <c r="N1" s="11"/>
-      <c r="O1" s="11"/>
-      <c r="P1" s="11"/>
+      <c r="B1" s="10"/>
+      <c r="C1" s="10"/>
+      <c r="D1" s="10"/>
+      <c r="E1" s="10"/>
+      <c r="F1" s="10"/>
+      <c r="G1" s="10"/>
+      <c r="H1" s="10"/>
+      <c r="I1" s="10"/>
+      <c r="J1" s="10"/>
+      <c r="K1" s="10"/>
+      <c r="L1" s="10"/>
+      <c r="M1" s="10"/>
+      <c r="N1" s="10"/>
+      <c r="O1" s="10"/>
+      <c r="P1" s="10"/>
       <c r="Q1" s="11"/>
-      <c r="R1" s="11"/>
-      <c r="S1" s="11"/>
-      <c r="T1" s="11"/>
-      <c r="U1" s="11"/>
-      <c r="V1" s="11"/>
-      <c r="W1" s="11"/>
-      <c r="X1" s="11"/>
-      <c r="Y1" s="11"/>
-      <c r="Z1" s="11"/>
-      <c r="AA1" s="11"/>
-      <c r="AB1" s="12"/>
     </row>
-    <row r="2" spans="1:94" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:83" x14ac:dyDescent="0.25">
       <c r="A2" s="8"/>
       <c r="B2" s="5" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="C2" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="E2" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="D2" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="E2" s="5" t="s">
+      <c r="F2" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="G2" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="H2" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="F2" s="5" t="s">
+      <c r="I2" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="G2" s="5" t="s">
+      <c r="J2" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="H2" s="5" t="s">
+      <c r="K2" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="I2" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="J2" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="K2" s="5" t="s">
-        <v>18</v>
-      </c>
       <c r="L2" s="5" t="s">
-        <v>19</v>
+        <v>7</v>
       </c>
       <c r="M2" s="5" t="s">
-        <v>20</v>
+        <v>8</v>
       </c>
       <c r="N2" s="5" t="s">
-        <v>21</v>
+        <v>9</v>
       </c>
       <c r="O2" s="5" t="s">
         <v>2</v>
       </c>
       <c r="P2" s="5" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="Q2" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="R2" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="S2" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="T2" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="U2" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="V2" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="W2" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="X2" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="Y2" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="Z2" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="AA2" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="AB2" s="5" t="s">
-        <v>10</v>
+        <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:94" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:83" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="9"/>
       <c r="B3" s="6"/>
       <c r="C3" s="6"/>
@@ -746,135 +626,50 @@
       <c r="O3" s="6"/>
       <c r="P3" s="6"/>
       <c r="Q3" s="6"/>
-      <c r="R3" s="6"/>
-      <c r="S3" s="6"/>
-      <c r="T3" s="6"/>
-      <c r="U3" s="6"/>
-      <c r="V3" s="6"/>
-      <c r="W3" s="6"/>
-      <c r="X3" s="6"/>
-      <c r="Y3" s="6"/>
-      <c r="Z3" s="6"/>
-      <c r="AA3" s="6"/>
-      <c r="AB3" s="6"/>
     </row>
-    <row r="4" spans="1:94" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:83" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>12345678</v>
       </c>
-      <c r="B4" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="E4" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="F4" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="G4" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="H4" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="I4" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="J4" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="K4" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="L4" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="M4" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="N4" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="O4" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="P4" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="Q4" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="R4" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="S4" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="T4" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="U4" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="V4" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="W4" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="X4" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="Y4" s="3"/>
-      <c r="Z4" s="3">
-        <v>4400</v>
-      </c>
-      <c r="AA4" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="AB4" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="BT4" s="2"/>
-      <c r="CP4" s="2"/>
+      <c r="B4" s="3"/>
+      <c r="C4" s="3"/>
+      <c r="D4" s="3"/>
+      <c r="E4" s="3"/>
+      <c r="F4" s="3"/>
+      <c r="G4" s="3"/>
+      <c r="H4" s="3"/>
+      <c r="I4" s="3"/>
+      <c r="J4" s="3"/>
+      <c r="K4" s="3"/>
+      <c r="L4" s="3"/>
+      <c r="M4" s="3"/>
+      <c r="N4" s="3"/>
+      <c r="O4" s="3"/>
+      <c r="P4" s="4"/>
+      <c r="Q4" s="4"/>
+      <c r="BI4" s="2"/>
+      <c r="CE4" s="2"/>
     </row>
   </sheetData>
-  <mergeCells count="29">
-    <mergeCell ref="AA2:AA3"/>
-    <mergeCell ref="R2:R3"/>
-    <mergeCell ref="Z2:Z3"/>
-    <mergeCell ref="N2:N3"/>
-    <mergeCell ref="K2:K3"/>
-    <mergeCell ref="H2:H3"/>
-    <mergeCell ref="Y2:Y3"/>
-    <mergeCell ref="T2:T3"/>
-    <mergeCell ref="S2:S3"/>
-    <mergeCell ref="X2:X3"/>
-    <mergeCell ref="W2:W3"/>
+  <mergeCells count="18">
     <mergeCell ref="Q2:Q3"/>
-    <mergeCell ref="V2:V3"/>
-    <mergeCell ref="AB2:AB3"/>
     <mergeCell ref="A1:A3"/>
-    <mergeCell ref="U2:U3"/>
     <mergeCell ref="L2:L3"/>
     <mergeCell ref="G2:G3"/>
-    <mergeCell ref="I2:I3"/>
+    <mergeCell ref="E2:E3"/>
+    <mergeCell ref="K2:K3"/>
     <mergeCell ref="J2:J3"/>
+    <mergeCell ref="H2:H3"/>
     <mergeCell ref="B2:B3"/>
+    <mergeCell ref="C2:C3"/>
+    <mergeCell ref="D2:D3"/>
+    <mergeCell ref="B1:Q1"/>
     <mergeCell ref="P2:P3"/>
     <mergeCell ref="O2:O3"/>
+    <mergeCell ref="N2:N3"/>
     <mergeCell ref="M2:M3"/>
-    <mergeCell ref="D2:D3"/>
-    <mergeCell ref="C2:C3"/>
-    <mergeCell ref="E2:E3"/>
+    <mergeCell ref="I2:I3"/>
     <mergeCell ref="F2:F3"/>
-    <mergeCell ref="B1:AB1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Update source for increase speed of tests
</commit_message>
<xml_diff>
--- a/TM/TestApp/_Files/Exel/TM.xlsx
+++ b/TM/TestApp/_Files/Exel/TM.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27231"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08E9AFBF-0077-410E-B87A-B25999F98DA7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2114EDEA-C820-4083-9D54-3EA6E601710C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5115" yWindow="3015" windowWidth="15375" windowHeight="7785" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4695" yWindow="1815" windowWidth="15375" windowHeight="7785" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TestResult" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="24">
   <si>
     <t>سریال دستگاه ها</t>
   </si>
@@ -40,15 +40,6 @@
     <t>ولتاژ 3.3 ولت</t>
   </si>
   <si>
-    <t xml:space="preserve">اتصال تغذیه 12 ولت </t>
-  </si>
-  <si>
-    <t>تنظیمات اعمال شده</t>
-  </si>
-  <si>
-    <t xml:space="preserve">اتصال تغذیه 220 ولت </t>
-  </si>
-  <si>
     <t>بررسی مدار Zero Cross</t>
   </si>
   <si>
@@ -70,12 +61,24 @@
     <t>ولتاز مودم</t>
   </si>
   <si>
-    <t>عملکرد مودم</t>
+    <t xml:space="preserve">اتصال تغذیه </t>
+  </si>
+  <si>
+    <t>تنظیمات برنامه پروگرم شده</t>
+  </si>
+  <si>
+    <t>ارتباط با سیم کارت</t>
   </si>
   <si>
     <t>OK</t>
   </si>
   <si>
+    <t>220v ac:0.05Amp 12v dc:11.72Volt</t>
+  </si>
+  <si>
+    <t>Chip:'196154487' Domain:'94.139.169.122:8000' Serial:'12345678' Prodoct:'1402-11-23'</t>
+  </si>
+  <si>
     <t>Power:OK, RS485:OK, NET1:OK, NET2:OK</t>
   </si>
   <si>
@@ -85,23 +88,17 @@
     <t>Reset:OK, Factory:OK</t>
   </si>
   <si>
-    <t>NO</t>
-  </si>
-  <si>
-    <t>Time = [1402/10/25 14:42:37] Device = [00310212345678] Domain = [94.139.169.122:8000]</t>
-  </si>
-  <si>
-    <t>66443B0CB575B3C9C98A673D94E695C7</t>
-  </si>
-  <si>
-    <t>v1.14021013</t>
+    <t>5F6FCEA73B0B0A331B2988D800CA0DBA</t>
+  </si>
+  <si>
+    <t>v1.14021121</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -120,13 +117,6 @@
       <b/>
       <sz val="18"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -225,7 +215,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -256,9 +246,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -541,36 +528,34 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:CE4"/>
+  <dimension ref="A1:CD4"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="Q8" sqref="Q8"/>
+      <selection pane="topRight" activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="26.140625" style="1" customWidth="1"/>
     <col min="2" max="2" width="14.5703125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="15.7109375" style="1" customWidth="1"/>
-    <col min="4" max="4" width="10.140625" style="1" customWidth="1"/>
-    <col min="5" max="5" width="10.7109375" style="1" customWidth="1"/>
-    <col min="6" max="6" width="8.42578125" style="1" customWidth="1"/>
-    <col min="7" max="7" width="12.5703125" style="1" customWidth="1"/>
-    <col min="8" max="8" width="13" style="1" customWidth="1"/>
-    <col min="9" max="9" width="11" style="1" customWidth="1"/>
-    <col min="10" max="10" width="12.42578125" style="1" customWidth="1"/>
-    <col min="11" max="11" width="15.140625" style="1" customWidth="1"/>
-    <col min="12" max="12" width="85" style="1" customWidth="1"/>
-    <col min="13" max="13" width="17.28515625" style="1" customWidth="1"/>
-    <col min="14" max="14" width="18" style="1" customWidth="1"/>
-    <col min="15" max="15" width="16" style="1" customWidth="1"/>
-    <col min="16" max="16" width="37.42578125" style="1" customWidth="1"/>
-    <col min="17" max="17" width="12.5703125" style="1" customWidth="1"/>
-    <col min="83" max="83" width="64" customWidth="1"/>
+    <col min="3" max="3" width="31.140625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="76.42578125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="33.5703125" style="1" customWidth="1"/>
+    <col min="6" max="6" width="37.140625" style="1" customWidth="1"/>
+    <col min="7" max="7" width="10.7109375" style="1" customWidth="1"/>
+    <col min="8" max="8" width="17.85546875" style="1" customWidth="1"/>
+    <col min="9" max="10" width="11" style="1" customWidth="1"/>
+    <col min="11" max="11" width="12.42578125" style="1" customWidth="1"/>
+    <col min="12" max="12" width="15.140625" style="1" customWidth="1"/>
+    <col min="13" max="13" width="21.28515625" style="1" customWidth="1"/>
+    <col min="14" max="14" width="16" style="1" customWidth="1"/>
+    <col min="15" max="15" width="37.42578125" style="1" customWidth="1"/>
+    <col min="16" max="16" width="12.5703125" style="1" customWidth="1"/>
+    <col min="82" max="82" width="64" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:83" ht="37.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:82" ht="37.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
@@ -588,61 +573,57 @@
       <c r="M1" s="10"/>
       <c r="N1" s="10"/>
       <c r="O1" s="10"/>
-      <c r="P1" s="10"/>
-      <c r="Q1" s="11"/>
+      <c r="P1" s="11"/>
     </row>
-    <row r="2" spans="1:83" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:82" x14ac:dyDescent="0.25">
       <c r="A2" s="8"/>
       <c r="B2" s="5" t="s">
         <v>1</v>
       </c>
       <c r="C2" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="E2" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="D2" s="5" t="s">
+      <c r="F2" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="G2" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="H2" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="I2" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="J2" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="K2" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="L2" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="M2" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="E2" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="F2" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="G2" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="H2" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="I2" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="J2" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="K2" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="L2" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="M2" s="5" t="s">
-        <v>8</v>
-      </c>
       <c r="N2" s="5" t="s">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="O2" s="5" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="P2" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="Q2" s="5" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:83" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:82" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="9"/>
       <c r="B3" s="6"/>
       <c r="C3" s="6"/>
@@ -659,14 +640,13 @@
       <c r="N3" s="6"/>
       <c r="O3" s="6"/>
       <c r="P3" s="6"/>
-      <c r="Q3" s="6"/>
     </row>
-    <row r="4" spans="1:83" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:82" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>12345678</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C4" s="3" t="s">
         <v>17</v>
@@ -675,67 +655,63 @@
         <v>18</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="H4" s="3" t="s">
         <v>20</v>
       </c>
       <c r="I4" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="J4" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="J4" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="K4" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="L4" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="M4" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="K4" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="L4" s="3" t="s">
+      <c r="N4" s="3">
+        <v>1700</v>
+      </c>
+      <c r="O4" s="4" t="s">
         <v>22</v>
-      </c>
-      <c r="M4" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="N4" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="O4" s="3">
-        <v>3600</v>
       </c>
       <c r="P4" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="Q4" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="BI4" s="2"/>
-      <c r="CE4" s="2"/>
+      <c r="BH4" s="2"/>
+      <c r="CD4" s="2"/>
     </row>
   </sheetData>
-  <mergeCells count="18">
+  <mergeCells count="17">
+    <mergeCell ref="N2:N3"/>
+    <mergeCell ref="M2:M3"/>
     <mergeCell ref="I2:I3"/>
-    <mergeCell ref="F2:F3"/>
-    <mergeCell ref="Q2:Q3"/>
+    <mergeCell ref="P2:P3"/>
     <mergeCell ref="A1:A3"/>
+    <mergeCell ref="H2:H3"/>
+    <mergeCell ref="G2:G3"/>
     <mergeCell ref="L2:L3"/>
-    <mergeCell ref="G2:G3"/>
-    <mergeCell ref="E2:E3"/>
     <mergeCell ref="K2:K3"/>
-    <mergeCell ref="J2:J3"/>
-    <mergeCell ref="H2:H3"/>
     <mergeCell ref="B2:B3"/>
     <mergeCell ref="C2:C3"/>
+    <mergeCell ref="F2:F3"/>
+    <mergeCell ref="B1:P1"/>
+    <mergeCell ref="O2:O3"/>
     <mergeCell ref="D2:D3"/>
-    <mergeCell ref="B1:Q1"/>
-    <mergeCell ref="P2:P3"/>
-    <mergeCell ref="O2:O3"/>
-    <mergeCell ref="N2:N3"/>
-    <mergeCell ref="M2:M3"/>
+    <mergeCell ref="E2:E3"/>
+    <mergeCell ref="J2:J3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Update stand down and up speed time
</commit_message>
<xml_diff>
--- a/TM/TestApp/_Files/Exel/TM.xlsx
+++ b/TM/TestApp/_Files/Exel/TM.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27231"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2114EDEA-C820-4083-9D54-3EA6E601710C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{530F5E2A-F06A-4903-80B3-9ED46F75D795}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4695" yWindow="1815" windowWidth="15375" windowHeight="7785" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="27">
   <si>
     <t>سریال دستگاه ها</t>
   </si>
@@ -73,12 +73,6 @@
     <t>OK</t>
   </si>
   <si>
-    <t>220v ac:0.05Amp 12v dc:11.72Volt</t>
-  </si>
-  <si>
-    <t>Chip:'196154487' Domain:'94.139.169.122:8000' Serial:'12345678' Prodoct:'1402-11-23'</t>
-  </si>
-  <si>
     <t>Power:OK, RS485:OK, NET1:OK, NET2:OK</t>
   </si>
   <si>
@@ -88,10 +82,25 @@
     <t>Reset:OK, Factory:OK</t>
   </si>
   <si>
-    <t>5F6FCEA73B0B0A331B2988D800CA0DBA</t>
-  </si>
-  <si>
     <t>v1.14021121</t>
+  </si>
+  <si>
+    <t>220v ac:0.07Amp 12v dc:11.70Volt</t>
+  </si>
+  <si>
+    <t>Chip:'196154487' Domain:'94.139.169.122:8000' Serial:'12345678' Prodoct:'1402-11-24'</t>
+  </si>
+  <si>
+    <t>264A2460CB7AED800865797C274D3CCA</t>
+  </si>
+  <si>
+    <t>220v ac:0.08Amp 12v dc:11.70Volt</t>
+  </si>
+  <si>
+    <t>Chip:'196154487' Domain:'94.139.169.122:8000' Serial:'87654321' Prodoct:'1402-11-24'</t>
+  </si>
+  <si>
+    <t>02A76906AA2DD0C23D47320C4A4E7996</t>
   </si>
 </sst>
 </file>
@@ -528,11 +537,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:CD4"/>
+  <dimension ref="A1:CD5"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="C6" sqref="C6"/>
+      <selection pane="topRight" activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -649,54 +658,102 @@
         <v>16</v>
       </c>
       <c r="C4" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="F4" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="D4" s="3" t="s">
+      <c r="G4" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="H4" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="E4" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="F4" s="3" t="s">
+      <c r="I4" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="J4" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="K4" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="L4" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="M4" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="G4" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="H4" s="3" t="s">
+      <c r="N4" s="3">
+        <v>1800</v>
+      </c>
+      <c r="O4" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="P4" s="4" t="s">
         <v>20</v>
-      </c>
-      <c r="I4" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="J4" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="K4" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="L4" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="M4" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="N4" s="3">
-        <v>1700</v>
-      </c>
-      <c r="O4" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="P4" s="4" t="s">
-        <v>23</v>
       </c>
       <c r="BH4" s="2"/>
       <c r="CD4" s="2"/>
     </row>
+    <row r="5" spans="1:82" x14ac:dyDescent="0.25">
+      <c r="A5" s="1">
+        <v>87654321</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="G5" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="I5" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="J5" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="K5" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="L5" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="M5" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="N5" s="1">
+        <v>1700</v>
+      </c>
+      <c r="O5" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="P5" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="17">
-    <mergeCell ref="N2:N3"/>
-    <mergeCell ref="M2:M3"/>
     <mergeCell ref="I2:I3"/>
     <mergeCell ref="P2:P3"/>
     <mergeCell ref="A1:A3"/>
@@ -712,6 +769,8 @@
     <mergeCell ref="D2:D3"/>
     <mergeCell ref="E2:E3"/>
     <mergeCell ref="J2:J3"/>
+    <mergeCell ref="N2:N3"/>
+    <mergeCell ref="M2:M3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>